<commit_message>
-  ( https://italent.cloudapp.net:9443/ccm/web/projects/iTalent#action=com.ibm.team.workitem.viewWorkItem&id= )
</commit_message>
<xml_diff>
--- a/italent/documents/analyse/use-cases/student/use_cases_student.xlsx
+++ b/italent/documents/analyse/use-cases/student/use_cases_student.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="46">
   <si>
     <t>Naam</t>
   </si>
@@ -159,29 +159,6 @@
 3. Systeem toont projecten en de aangemeldde gebruikersgegevens</t>
   </si>
   <si>
-    <t>Project toevoegen</t>
-  </si>
-  <si>
-    <t>Nieuw project toevoegen</t>
-  </si>
-  <si>
-    <t>Er werd een nieuw project toegevoegd</t>
-  </si>
-  <si>
-    <t>[Gebruiker annuleert toevoegen]
-1. Gebruiker klikt op knop 'annuleren'
-2. Systeem laat projectenlijst zien (ref. use case 'Projectenlijst tonen')</t>
-  </si>
-  <si>
-    <t>1. Gebruiker druk op een knop op een nieuw project toe te voegen
-2. Gebruiker voert een titel, beschrijving, begin- en einddatum in
-3. Gebruiker kiest een categorie (ref. use case 'Categorie kiezen')
-4. Gebruiker voegt eventueel documenten toe (ref. use case 'Documenten toevoegen')
-5. Gebruiker voegt eventueel foto(s) toe (ref. use case 'Foto toevoegen')
-6. Gebruiker voegt eventueel video(s) toe (ref. use case 'Video toevoegen')
-7. Gebruiker voert aantal subscribers in met hun type (ref. use case 'subscribertypes toevoegen')</t>
-  </si>
-  <si>
     <t>Aanmelden</t>
   </si>
   <si>
@@ -191,103 +168,10 @@
     <t>use case 'aanmelden' werd successvol afgerond of er is een actieve sessie voor de gebruiker</t>
   </si>
   <si>
-    <t>Gebruiker kiest een category voor het nieuwe project</t>
-  </si>
-  <si>
-    <t>Gebruiker voegt documenten toe aan project</t>
-  </si>
-  <si>
-    <t>Gebruiker voegt videos toe aan project</t>
-  </si>
-  <si>
-    <t>Gebruiker voegt fotos toe aan project</t>
-  </si>
-  <si>
-    <t>Gebruiker voegt subscribertypes toe aan project</t>
-  </si>
-  <si>
-    <t>Documenten bewerken</t>
-  </si>
-  <si>
-    <t>Foto bewerken</t>
-  </si>
-  <si>
-    <t>Video bewerken</t>
-  </si>
-  <si>
-    <t>Subscribertypes bewerken</t>
-  </si>
-  <si>
-    <t>Categorie bewerken</t>
-  </si>
-  <si>
-    <t>Project bewerken</t>
-  </si>
-  <si>
-    <t>use case 'Projecten toevoegen' of 'Projecten beheren' wordt uitgevoerd tot en met referentie naar deze use case</t>
-  </si>
-  <si>
-    <t>Subscribertype werd gekozen voor bepaald project</t>
-  </si>
-  <si>
-    <t>1. Systeem toont invoerveld om foto-URL toe te voegen
-2. Gebruiker voert fotolocatie in
-3. Systeem valideert invoer
-4. Systeem geeft controle terug aan parent- use case</t>
-  </si>
-  <si>
-    <t>1. Systeem laad mogelijke categorieen
-2. Gebruiker kieset categorie
-3. Systeem geeft controle terug aan parent- use case</t>
-  </si>
-  <si>
-    <t>1. Systeem toont invoerveld om document-URL toe te voegen
-2. Gebruiker voert documentlocatie in
-3. Systeem valideert invoer
-4. Systeem geeft controle terug aan parent- use case</t>
-  </si>
-  <si>
-    <t>[invoervalidatie mislukt]
-1. Systeem toont melding "URL is niet correct"
-2. Systeem maakt invoer leeg en geeft controle terug aan de gebruiker</t>
-  </si>
-  <si>
-    <t>Document toegevoegd/bewerkt</t>
-  </si>
-  <si>
-    <t>Categorie toegevoegd/bewerkt</t>
-  </si>
-  <si>
-    <t>foto toegevoegd/bewerkt</t>
-  </si>
-  <si>
-    <t>video toegevoegd/bewerkt</t>
-  </si>
-  <si>
-    <t>1. Systeem toont invoerveld om video-URL toe te voegen via youtube
-2. Gebruiker voert videolocatie in
-3. Systeem valideert invoer
-4. Systeem geeft controle terug aan parent- use case</t>
-  </si>
-  <si>
-    <t>1. Systeem toont invoerveld om subscribertype toe te voegen
-2. Gebruiker kiest een type (Health/IT/…)
-3. Systeem geeft controle terug aan parent- use case</t>
-  </si>
-  <si>
     <t>Bestaand project aanpassen</t>
   </si>
   <si>
     <t>Bestaande PXL student die het project heeft aangemaakt / docent die is ingeschreven voor het project</t>
-  </si>
-  <si>
-    <t>1. Gebruiker druk op een knop op een bestaand project aan te passen
-2. Gebruiker voert een titel, beschrijving, begin- en einddatum in
-3. Gebruiker kiest een categorie (ref. use case 'Categorie kiezen')
-4. Gebruiker voegt eventueel documenten toe (ref. use case 'Documenten toevoegen')
-5. Gebruiker voegt eventueel foto(s) toe (ref. use case 'Foto toevoegen')
-6. Gebruiker voegt eventueel video(s) toe (ref. use case 'Video toevoegen')
-7. Gebruiker voert aantal subscribers in met hun type (ref. use case 'subscribertypes toevoegen')</t>
   </si>
   <si>
     <t>Er werd een bestaand project aangepast</t>
@@ -296,6 +180,18 @@
     <t>[Gebruiker annuleert aanpassing]
 1. Gebruiker klikt op knop 'annuleren'
 2. Systeem laat projectenlijst zien (ref. use case 'Projectenlijst tonen')</t>
+  </si>
+  <si>
+    <t>Project toevoegen/bewerken</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Gebruiker druk op een knop op een bestaand project aan te passen
+2. Gebruiker voert een titel, beschrijving, begin- en einddatum in
+3. Gebruiker kiest een categorie
+4. Gebruiker voegt eventueel documenten toe
+5. Gebruiker voegt eventueel foto(s) toe 
+6. Gebruiker voegt eventueel video(s) toe 
+7. Gebruiker voert aantal subscribers in met hun type </t>
   </si>
 </sst>
 </file>
@@ -752,10 +648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:D118"/>
+  <dimension ref="C2:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B104" workbookViewId="0">
-      <selection activeCell="D121" sqref="D121"/>
+    <sheetView tabSelected="1" topLeftCell="B46" workbookViewId="0">
+      <selection activeCell="B57" sqref="A57:XFD57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,7 +666,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="3:4" x14ac:dyDescent="0.25">
@@ -818,7 +714,7 @@
         <v>6</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="3:4" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -867,7 +763,7 @@
         <v>4</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.25">
@@ -1158,7 +1054,7 @@
         <v>0</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="58" spans="3:4" x14ac:dyDescent="0.25">
@@ -1174,7 +1070,7 @@
         <v>2</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="60" spans="3:4" x14ac:dyDescent="0.25">
@@ -1182,7 +1078,7 @@
         <v>3</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
     </row>
     <row r="61" spans="3:4" x14ac:dyDescent="0.25">
@@ -1198,7 +1094,7 @@
         <v>5</v>
       </c>
       <c r="D62" s="10" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="63" spans="3:4" x14ac:dyDescent="0.25">
@@ -1206,7 +1102,7 @@
         <v>6</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="64" spans="3:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1214,393 +1110,7 @@
         <v>7</v>
       </c>
       <c r="D64" s="11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="65" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="66" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C66" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="67" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C67" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D67" s="5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="68" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C68" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D68" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="69" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C69" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="70" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C70" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D70" s="9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="71" spans="3:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="C71" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D71" s="10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="72" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C72" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D72" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="73" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C73" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D73" s="11"/>
-    </row>
-    <row r="74" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="75" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C75" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="76" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C76" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D76" s="5">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="77" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C77" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D77" s="7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="78" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C78" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D78" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="79" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C79" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D79" s="9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="80" spans="3:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="C80" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D80" s="10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="81" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C81" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D81" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="82" spans="3:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C82" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D82" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="83" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="84" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C84" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D84" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="85" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C85" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D85" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="86" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C86" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D86" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="87" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C87" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D87" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="88" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C88" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D88" s="9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="89" spans="3:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="C89" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D89" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="90" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C90" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D90" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="91" spans="3:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C91" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D91" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="92" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="93" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C93" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D93" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="94" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C94" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D94" s="5">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="95" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C95" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D95" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="96" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C96" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D96" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="97" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C97" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D97" s="9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="98" spans="3:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="C98" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D98" s="10" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="99" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C99" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D99" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="100" spans="3:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C100" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D100" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="101" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="102" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C102" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D102" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="103" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C103" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D103" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="104" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C104" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D104" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="105" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C105" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D105" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="106" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C106" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D106" s="9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="107" spans="3:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="C107" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D107" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="108" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C108" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D108" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="109" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C109" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D109" s="11"/>
-    </row>
-    <row r="110" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="111" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C111" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D111" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="112" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C112" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D112" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="113" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C113" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D113" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="114" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C114" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D114" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="115" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C115" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D115" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="116" spans="3:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="C116" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D116" s="10" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="117" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C117" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D117" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="118" spans="3:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C118" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D118" s="11" t="s">
-        <v>72</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>